<commit_message>
Final 6/12:Completed Simple,medium,Complex Test cases. It can be run in single testng.xml file.Uploaded the excel files with results and defects.
</commit_message>
<xml_diff>
--- a/final-framework-testng/Signup_Student.xlsx
+++ b/final-framework-testng/Signup_Student.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A13D90-324B-4F6A-BBF6-FAB2E81D6CC6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35D8B8C-9C90-491B-A30A-4DA852FDEC1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,16 +79,16 @@
     <t>Test8@123</t>
   </si>
   <si>
-    <t>TestSignupa17</t>
-  </si>
-  <si>
-    <t>TestSignupa14</t>
-  </si>
-  <si>
-    <t>TestSignupa15</t>
-  </si>
-  <si>
-    <t>TestSignupa16</t>
+    <t>TestSignupc17</t>
+  </si>
+  <si>
+    <t>TestSignupc14</t>
+  </si>
+  <si>
+    <t>TestSignupc15</t>
+  </si>
+  <si>
+    <t>TestSignupc16</t>
   </si>
 </sst>
 </file>

</xml_diff>